<commit_message>
Se agregó servicio de filtrado para administrador
</commit_message>
<xml_diff>
--- a/Lealtad-Dominio/src/test/resources/FORD.xlsx
+++ b/Lealtad-Dominio/src/test/resources/FORD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10005" windowHeight="5355" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15225" windowHeight="6345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$O$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$B$2:$P$110</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <oleSize ref="A1:H16"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A16:L34"/>
 </workbook>
 </file>
 
@@ -1613,9 +1613,6 @@
     <t xml:space="preserve"> $5,500.00 </t>
   </si>
   <si>
-    <t>000987739</t>
-  </si>
-  <si>
     <t xml:space="preserve"> $16,000.00 </t>
   </si>
   <si>
@@ -1634,9 +1631,6 @@
     <t>94.3</t>
   </si>
   <si>
-    <t>000972575</t>
-  </si>
-  <si>
     <t xml:space="preserve">85 </t>
   </si>
   <si>
@@ -1652,9 +1646,6 @@
     <t>88</t>
   </si>
   <si>
-    <t>000967675</t>
-  </si>
-  <si>
     <t xml:space="preserve">34 </t>
   </si>
   <si>
@@ -1673,9 +1664,6 @@
     <t>94.7</t>
   </si>
   <si>
-    <t>000983357</t>
-  </si>
-  <si>
     <t xml:space="preserve">54 </t>
   </si>
   <si>
@@ -1694,9 +1682,6 @@
     <t>100</t>
   </si>
   <si>
-    <t>001044079</t>
-  </si>
-  <si>
     <t xml:space="preserve">49 </t>
   </si>
   <si>
@@ -2871,6 +2856,21 @@
   </si>
   <si>
     <t>43.3</t>
+  </si>
+  <si>
+    <t>123456781</t>
+  </si>
+  <si>
+    <t>123456782</t>
+  </si>
+  <si>
+    <t>123456783</t>
+  </si>
+  <si>
+    <t>123456784</t>
+  </si>
+  <si>
+    <t>123456785</t>
   </si>
 </sst>
 </file>
@@ -2906,15 +2906,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -8344,13 +8353,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AT110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="D102" workbookViewId="0">
+      <selection activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="46" width="11.42578125" style="1"/>
+    <col min="2" max="11" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="16.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24" style="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="1" customWidth="1"/>
+    <col min="15" max="46" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16">
@@ -8575,8 +8588,8 @@
       <c r="L6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>530</v>
+      <c r="M6" s="2" t="s">
+        <v>945</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>27</v>
@@ -8585,7 +8598,7 @@
         <v>28</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7" spans="2:16">
@@ -8596,25 +8609,25 @@
         <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>535</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>529</v>
@@ -8622,8 +8635,8 @@
       <c r="L7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>537</v>
+      <c r="M7" s="2" t="s">
+        <v>946</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>32</v>
@@ -8632,7 +8645,7 @@
         <v>33</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="2:16">
@@ -8643,25 +8656,25 @@
         <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>529</v>
@@ -8669,8 +8682,8 @@
       <c r="L8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>543</v>
+      <c r="M8" s="2" t="s">
+        <v>947</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>37</v>
@@ -8679,7 +8692,7 @@
         <v>38</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="9" spans="2:16">
@@ -8690,25 +8703,25 @@
         <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>548</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>529</v>
@@ -8716,8 +8729,8 @@
       <c r="L9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>550</v>
+      <c r="M9" s="2" t="s">
+        <v>948</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>42</v>
@@ -8726,7 +8739,7 @@
         <v>43</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -8737,25 +8750,25 @@
         <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>555</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>529</v>
@@ -8763,8 +8776,8 @@
       <c r="L10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>557</v>
+      <c r="M10" s="2" t="s">
+        <v>949</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>47</v>
@@ -8773,7 +8786,7 @@
         <v>48</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="2:16">
@@ -8784,25 +8797,25 @@
         <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>529</v>
@@ -8811,7 +8824,7 @@
         <v>51</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>47</v>
@@ -8820,7 +8833,7 @@
         <v>52</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="12" spans="2:16">
@@ -8831,25 +8844,25 @@
         <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>529</v>
@@ -8858,7 +8871,7 @@
         <v>55</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>56</v>
@@ -8867,7 +8880,7 @@
         <v>57</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13" spans="2:16">
@@ -8878,25 +8891,25 @@
         <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>529</v>
@@ -8905,7 +8918,7 @@
         <v>60</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>61</v>
@@ -8914,7 +8927,7 @@
         <v>62</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14" spans="2:16">
@@ -8925,25 +8938,25 @@
         <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>17</v>
@@ -8952,7 +8965,7 @@
         <v>65</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>66</v>
@@ -8972,25 +8985,25 @@
         <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>17</v>
@@ -8999,7 +9012,7 @@
         <v>70</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>71</v>
@@ -9019,25 +9032,25 @@
         <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>523</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>529</v>
@@ -9046,7 +9059,7 @@
         <v>75</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>76</v>
@@ -9055,7 +9068,7 @@
         <v>77</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -9066,25 +9079,25 @@
         <v>79</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>529</v>
@@ -9093,7 +9106,7 @@
         <v>80</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>81</v>
@@ -9102,7 +9115,7 @@
         <v>82</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -9113,25 +9126,25 @@
         <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>529</v>
@@ -9140,7 +9153,7 @@
         <v>85</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>86</v>
@@ -9149,7 +9162,7 @@
         <v>87</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="2:16">
@@ -9160,25 +9173,25 @@
         <v>89</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>529</v>
@@ -9187,7 +9200,7 @@
         <v>90</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>91</v>
@@ -9196,7 +9209,7 @@
         <v>92</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="20" spans="2:16">
@@ -9207,25 +9220,25 @@
         <v>94</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>529</v>
@@ -9234,7 +9247,7 @@
         <v>95</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>96</v>
@@ -9243,7 +9256,7 @@
         <v>97</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="2:16">
@@ -9254,25 +9267,25 @@
         <v>99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>529</v>
@@ -9281,7 +9294,7 @@
         <v>100</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>101</v>
@@ -9290,7 +9303,7 @@
         <v>102</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="22" spans="2:16">
@@ -9301,25 +9314,25 @@
         <v>104</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>527</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>529</v>
@@ -9328,7 +9341,7 @@
         <v>105</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>106</v>
@@ -9337,7 +9350,7 @@
         <v>107</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="23" spans="2:16">
@@ -9348,34 +9361,34 @@
         <v>109</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>621</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>110</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>111</v>
@@ -9384,7 +9397,7 @@
         <v>112</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -9395,34 +9408,34 @@
         <v>114</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>115</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>116</v>
@@ -9431,7 +9444,7 @@
         <v>117</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -9442,34 +9455,34 @@
         <v>119</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>635</v>
-      </c>
       <c r="K25" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>120</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>121</v>
@@ -9478,7 +9491,7 @@
         <v>122</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -9489,34 +9502,34 @@
         <v>124</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>638</v>
-      </c>
       <c r="K26" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>125</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>126</v>
@@ -9525,7 +9538,7 @@
         <v>127</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -9536,34 +9549,34 @@
         <v>129</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>130</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>131</v>
@@ -9572,7 +9585,7 @@
         <v>132</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -9589,28 +9602,28 @@
         <v>523</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>135</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>47</v>
@@ -9619,7 +9632,7 @@
         <v>136</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="29" spans="2:16">
@@ -9630,34 +9643,34 @@
         <v>138</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>139</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>140</v>
@@ -9666,7 +9679,7 @@
         <v>141</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="30" spans="2:16">
@@ -9677,34 +9690,34 @@
         <v>143</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>144</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>145</v>
@@ -9713,7 +9726,7 @@
         <v>146</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -9724,25 +9737,25 @@
         <v>148</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>17</v>
@@ -9751,7 +9764,7 @@
         <v>149</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>150</v>
@@ -9771,25 +9784,25 @@
         <v>153</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>17</v>
@@ -9798,7 +9811,7 @@
         <v>154</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>61</v>
@@ -9818,25 +9831,25 @@
         <v>157</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>17</v>
@@ -9845,7 +9858,7 @@
         <v>158</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>27</v>
@@ -9865,34 +9878,34 @@
         <v>161</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>162</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>163</v>
@@ -9901,7 +9914,7 @@
         <v>164</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="35" spans="2:16">
@@ -9912,34 +9925,34 @@
         <v>166</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>167</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>168</v>
@@ -9948,7 +9961,7 @@
         <v>169</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="36" spans="2:16">
@@ -9959,34 +9972,34 @@
         <v>171</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>172</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>173</v>
@@ -9995,7 +10008,7 @@
         <v>174</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="37" spans="2:16">
@@ -10006,34 +10019,34 @@
         <v>176</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>177</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>91</v>
@@ -10042,7 +10055,7 @@
         <v>178</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="38" spans="2:16">
@@ -10053,34 +10066,34 @@
         <v>180</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>181</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>182</v>
@@ -10089,7 +10102,7 @@
         <v>183</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="39" spans="2:16">
@@ -10100,34 +10113,34 @@
         <v>185</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>186</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>187</v>
@@ -10136,7 +10149,7 @@
         <v>188</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="40" spans="2:16">
@@ -10147,34 +10160,34 @@
         <v>190</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>191</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>192</v>
@@ -10183,7 +10196,7 @@
         <v>193</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="41" spans="2:16">
@@ -10194,34 +10207,34 @@
         <v>195</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>196</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>197</v>
@@ -10230,7 +10243,7 @@
         <v>198</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="42" spans="2:16">
@@ -10241,34 +10254,34 @@
         <v>200</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>201</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>27</v>
@@ -10277,7 +10290,7 @@
         <v>202</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="43" spans="2:16">
@@ -10288,34 +10301,34 @@
         <v>204</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>205</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>206</v>
@@ -10324,7 +10337,7 @@
         <v>207</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="44" spans="2:16">
@@ -10335,25 +10348,25 @@
         <v>209</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>17</v>
@@ -10362,7 +10375,7 @@
         <v>210</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>211</v>
@@ -10382,34 +10395,34 @@
         <v>214</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>529</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>215</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>216</v>
@@ -10418,7 +10431,7 @@
         <v>217</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="46" spans="2:16">
@@ -10429,34 +10442,34 @@
         <v>219</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>716</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>220</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>145</v>
@@ -10465,7 +10478,7 @@
         <v>221</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="47" spans="2:16">
@@ -10476,25 +10489,25 @@
         <v>223</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>524</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>17</v>
@@ -10503,7 +10516,7 @@
         <v>224</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>225</v>
@@ -10512,7 +10525,7 @@
         <v>226</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="48" spans="2:16">
@@ -10523,34 +10536,34 @@
         <v>228</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>229</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>230</v>
@@ -10559,7 +10572,7 @@
         <v>231</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="49" spans="2:16">
@@ -10570,25 +10583,25 @@
         <v>233</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>17</v>
@@ -10597,7 +10610,7 @@
         <v>234</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>235</v>
@@ -10606,7 +10619,7 @@
         <v>236</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="50" spans="2:16">
@@ -10617,25 +10630,25 @@
         <v>238</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>17</v>
@@ -10644,7 +10657,7 @@
         <v>239</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="N50" s="1" t="s">
         <v>145</v>
@@ -10653,7 +10666,7 @@
         <v>240</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="51" spans="2:16">
@@ -10664,25 +10677,25 @@
         <v>242</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="H51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>737</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>17</v>
@@ -10691,7 +10704,7 @@
         <v>243</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>244</v>
@@ -10700,7 +10713,7 @@
         <v>245</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="52" spans="2:16">
@@ -10711,25 +10724,25 @@
         <v>247</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>17</v>
@@ -10738,7 +10751,7 @@
         <v>248</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>249</v>
@@ -10747,7 +10760,7 @@
         <v>250</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="53" spans="2:16">
@@ -10758,34 +10771,34 @@
         <v>252</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>253</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>254</v>
@@ -10794,7 +10807,7 @@
         <v>255</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="54" spans="2:16">
@@ -10805,34 +10818,34 @@
         <v>257</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>258</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>259</v>
@@ -10841,7 +10854,7 @@
         <v>260</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="55" spans="2:16">
@@ -10852,25 +10865,25 @@
         <v>262</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>17</v>
@@ -10879,7 +10892,7 @@
         <v>263</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>264</v>
@@ -10888,7 +10901,7 @@
         <v>265</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="56" spans="2:16">
@@ -10899,25 +10912,25 @@
         <v>267</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>17</v>
@@ -10926,7 +10939,7 @@
         <v>268</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>96</v>
@@ -10946,25 +10959,25 @@
         <v>271</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>17</v>
@@ -10973,7 +10986,7 @@
         <v>272</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>273</v>
@@ -10993,25 +11006,25 @@
         <v>276</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>17</v>
@@ -11020,7 +11033,7 @@
         <v>277</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>278</v>
@@ -11040,25 +11053,25 @@
         <v>281</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>17</v>
@@ -11067,7 +11080,7 @@
         <v>282</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>283</v>
@@ -11087,25 +11100,25 @@
         <v>286</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>17</v>
@@ -11114,7 +11127,7 @@
         <v>287</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>145</v>
@@ -11134,25 +11147,25 @@
         <v>290</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>17</v>
@@ -11161,7 +11174,7 @@
         <v>291</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="N61" s="1" t="s">
         <v>292</v>
@@ -11181,25 +11194,25 @@
         <v>295</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>17</v>
@@ -11208,7 +11221,7 @@
         <v>296</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>297</v>
@@ -11228,25 +11241,25 @@
         <v>300</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>17</v>
@@ -11255,7 +11268,7 @@
         <v>301</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="N63" s="1" t="s">
         <v>302</v>
@@ -11275,25 +11288,25 @@
         <v>305</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>17</v>
@@ -11302,7 +11315,7 @@
         <v>306</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="N64" s="1" t="s">
         <v>307</v>
@@ -11322,25 +11335,25 @@
         <v>310</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>17</v>
@@ -11349,7 +11362,7 @@
         <v>311</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>312</v>
@@ -11369,25 +11382,25 @@
         <v>315</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>17</v>
@@ -11396,7 +11409,7 @@
         <v>316</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="N66" s="1" t="s">
         <v>317</v>
@@ -11416,25 +11429,25 @@
         <v>320</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>17</v>
@@ -11443,7 +11456,7 @@
         <v>321</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="N67" s="1" t="s">
         <v>322</v>
@@ -11463,25 +11476,25 @@
         <v>325</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>17</v>
@@ -11490,7 +11503,7 @@
         <v>326</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>81</v>
@@ -11510,25 +11523,25 @@
         <v>329</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>17</v>
@@ -11537,7 +11550,7 @@
         <v>330</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>331</v>
@@ -11557,25 +11570,25 @@
         <v>334</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="G70" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J70" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>807</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>17</v>
@@ -11584,7 +11597,7 @@
         <v>335</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>336</v>
@@ -11604,25 +11617,25 @@
         <v>339</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>17</v>
@@ -11631,7 +11644,7 @@
         <v>340</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>341</v>
@@ -11651,25 +11664,25 @@
         <v>344</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>17</v>
@@ -11678,7 +11691,7 @@
         <v>345</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="N72" s="1" t="s">
         <v>346</v>
@@ -11698,25 +11711,25 @@
         <v>349</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>17</v>
@@ -11725,7 +11738,7 @@
         <v>350</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="N73" s="1" t="s">
         <v>27</v>
@@ -11745,25 +11758,25 @@
         <v>353</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>17</v>
@@ -11772,7 +11785,7 @@
         <v>354</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="N74" s="1" t="s">
         <v>355</v>
@@ -11792,25 +11805,25 @@
         <v>358</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="G75" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J75" s="1" t="s">
         <v>817</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J75" s="1" t="s">
-        <v>822</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>17</v>
@@ -11819,7 +11832,7 @@
         <v>359</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="N75" s="1" t="s">
         <v>360</v>
@@ -11839,25 +11852,25 @@
         <v>363</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>17</v>
@@ -11866,7 +11879,7 @@
         <v>364</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="N76" s="1" t="s">
         <v>365</v>
@@ -11886,25 +11899,25 @@
         <v>368</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>17</v>
@@ -11913,7 +11926,7 @@
         <v>369</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="N77" s="1" t="s">
         <v>121</v>
@@ -11933,25 +11946,25 @@
         <v>372</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>17</v>
@@ -11960,7 +11973,7 @@
         <v>373</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
       <c r="N78" s="1" t="s">
         <v>374</v>
@@ -11980,25 +11993,25 @@
         <v>376</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="G79" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" s="1" t="s">
         <v>833</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>834</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>838</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>17</v>
@@ -12007,7 +12020,7 @@
         <v>377</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>378</v>
@@ -12027,25 +12040,25 @@
         <v>381</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>17</v>
@@ -12054,7 +12067,7 @@
         <v>382</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="N80" s="1" t="s">
         <v>383</v>
@@ -12074,25 +12087,25 @@
         <v>386</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>17</v>
@@ -12101,7 +12114,7 @@
         <v>387</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="N81" s="1" t="s">
         <v>27</v>
@@ -12121,25 +12134,25 @@
         <v>390</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>17</v>
@@ -12148,7 +12161,7 @@
         <v>391</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>392</v>
@@ -12168,25 +12181,25 @@
         <v>395</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>17</v>
@@ -12195,7 +12208,7 @@
         <v>396</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>397</v>
@@ -12215,25 +12228,25 @@
         <v>400</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>17</v>
@@ -12242,7 +12255,7 @@
         <v>401</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
       <c r="N84" s="1" t="s">
         <v>402</v>
@@ -12262,25 +12275,25 @@
         <v>405</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>17</v>
@@ -12289,7 +12302,7 @@
         <v>406</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="N85" s="1" t="s">
         <v>407</v>
@@ -12309,25 +12322,25 @@
         <v>410</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>17</v>
@@ -12336,7 +12349,7 @@
         <v>411</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="N86" s="1" t="s">
         <v>96</v>
@@ -12356,25 +12369,25 @@
         <v>414</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>17</v>
@@ -12383,7 +12396,7 @@
         <v>415</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>416</v>
@@ -12403,25 +12416,25 @@
         <v>419</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>17</v>
@@ -12430,7 +12443,7 @@
         <v>420</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="N88" s="1" t="s">
         <v>91</v>
@@ -12450,25 +12463,25 @@
         <v>423</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>17</v>
@@ -12477,7 +12490,7 @@
         <v>424</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
       <c r="N89" s="1" t="s">
         <v>425</v>
@@ -12497,25 +12510,25 @@
         <v>428</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>17</v>
@@ -12524,7 +12537,7 @@
         <v>429</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="N90" s="1" t="s">
         <v>392</v>
@@ -12544,25 +12557,25 @@
         <v>432</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
       <c r="K91" s="1" t="s">
         <v>17</v>
@@ -12571,7 +12584,7 @@
         <v>433</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>881</v>
+        <v>876</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>434</v>
@@ -12591,25 +12604,25 @@
         <v>437</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>885</v>
+        <v>880</v>
       </c>
       <c r="K92" s="1" t="s">
         <v>17</v>
@@ -12618,7 +12631,7 @@
         <v>438</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>886</v>
+        <v>881</v>
       </c>
       <c r="N92" s="1" t="s">
         <v>168</v>
@@ -12638,25 +12651,25 @@
         <v>441</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>888</v>
+        <v>883</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>889</v>
+        <v>884</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>17</v>
@@ -12665,7 +12678,7 @@
         <v>442</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>890</v>
+        <v>885</v>
       </c>
       <c r="N93" s="1" t="s">
         <v>443</v>
@@ -12685,25 +12698,25 @@
         <v>446</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>891</v>
+        <v>886</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>17</v>
@@ -12712,7 +12725,7 @@
         <v>447</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="N94" s="1" t="s">
         <v>448</v>
@@ -12732,25 +12745,25 @@
         <v>451</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>17</v>
@@ -12759,7 +12772,7 @@
         <v>452</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="N95" s="1" t="s">
         <v>145</v>
@@ -12779,25 +12792,25 @@
         <v>455</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>17</v>
@@ -12806,7 +12819,7 @@
         <v>456</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
       <c r="N96" s="1" t="s">
         <v>457</v>
@@ -12826,25 +12839,25 @@
         <v>460</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
       <c r="G97" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J97" s="1" t="s">
         <v>898</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>899</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J97" s="1" t="s">
-        <v>903</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>17</v>
@@ -12853,7 +12866,7 @@
         <v>461</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="N97" s="1" t="s">
         <v>96</v>
@@ -12873,25 +12886,25 @@
         <v>464</v>
       </c>
       <c r="D98" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>630</v>
-      </c>
       <c r="G98" s="1" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>17</v>
@@ -12900,7 +12913,7 @@
         <v>465</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="N98" s="1" t="s">
         <v>145</v>
@@ -12920,25 +12933,25 @@
         <v>468</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="K99" s="1" t="s">
         <v>17</v>
@@ -12947,7 +12960,7 @@
         <v>469</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="N99" s="1" t="s">
         <v>81</v>
@@ -12967,25 +12980,25 @@
         <v>472</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
       <c r="K100" s="1" t="s">
         <v>17</v>
@@ -12994,7 +13007,7 @@
         <v>473</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>915</v>
+        <v>910</v>
       </c>
       <c r="N100" s="1" t="s">
         <v>244</v>
@@ -13014,25 +13027,25 @@
         <v>476</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>17</v>
@@ -13041,7 +13054,7 @@
         <v>477</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="N101" s="1" t="s">
         <v>360</v>
@@ -13061,25 +13074,25 @@
         <v>480</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>17</v>
@@ -13108,25 +13121,25 @@
         <v>483</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>17</v>
@@ -13135,7 +13148,7 @@
         <v>484</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
       <c r="N103" s="1" t="s">
         <v>145</v>
@@ -13155,25 +13168,25 @@
         <v>487</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>923</v>
+        <v>918</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>17</v>
@@ -13182,7 +13195,7 @@
         <v>488</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
       <c r="N104" s="1" t="s">
         <v>187</v>
@@ -13202,19 +13215,19 @@
         <v>491</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>927</v>
+        <v>922</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>929</v>
+        <v>924</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>17</v>
@@ -13249,25 +13262,25 @@
         <v>494</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>930</v>
+        <v>925</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>930</v>
+        <v>925</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>17</v>
@@ -13276,7 +13289,7 @@
         <v>495</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="N106" s="1" t="s">
         <v>392</v>
@@ -13296,25 +13309,25 @@
         <v>498</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>17</v>
@@ -13323,7 +13336,7 @@
         <v>499</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
       <c r="N107" s="1" t="s">
         <v>500</v>
@@ -13343,25 +13356,25 @@
         <v>503</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>939</v>
+        <v>934</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>17</v>
@@ -13370,7 +13383,7 @@
         <v>504</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>942</v>
+        <v>937</v>
       </c>
       <c r="N108" s="1" t="s">
         <v>505</v>
@@ -13390,19 +13403,19 @@
         <v>508</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>943</v>
+        <v>938</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>944</v>
+        <v>939</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>17</v>
@@ -13417,7 +13430,7 @@
         <v>509</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="N109" s="1" t="s">
         <v>510</v>
@@ -13437,25 +13450,25 @@
         <v>513</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>946</v>
+        <v>941</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>948</v>
+        <v>943</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>949</v>
+        <v>944</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>17</v>
@@ -13478,7 +13491,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>